<commit_message>
Added button that gives suggestions for where to put people
</commit_message>
<xml_diff>
--- a/Sample Spreadsheets/Spreadsheet.xlsx
+++ b/Sample Spreadsheets/Spreadsheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
   <si>
     <t>Your Name</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>Steven T</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -421,7 +424,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -541,7 +544,7 @@
         <v>17</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added multiple boat capabilities.
Dragging and dropping needs additional logic now.
</commit_message>
<xml_diff>
--- a/Sample Spreadsheets/Spreadsheet.xlsx
+++ b/Sample Spreadsheets/Spreadsheet.xlsx
@@ -16,9 +16,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
   <si>
-    <t>Your Name</t>
-  </si>
-  <si>
     <t>Yes, and I can drive.</t>
   </si>
   <si>
@@ -80,6 +77,9 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Your name (including last initial):</t>
   </si>
 </sst>
 </file>
@@ -424,159 +424,159 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>